<commit_message>
Báo cáo tuần 3
</commit_message>
<xml_diff>
--- a/Report/ThuyThaWBS.xlsx
+++ b/Report/ThuyThaWBS.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="87">
   <si>
     <t>○</t>
     <phoneticPr fontId="5"/>
@@ -289,9 +289,6 @@
     <t>thiết kế giao diện trang web đơn giản</t>
   </si>
   <si>
-    <t>chưa làm kịp thể loại, quốc gia</t>
-  </si>
-  <si>
     <t>test lỗi, làm báo cáo đề tài TTTN.</t>
   </si>
   <si>
@@ -353,6 +350,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Quản lý bài hát trực tuyến : thêm, xóa, sửa bài hát</t>
+  </si>
+  <si>
+    <t>đã phân loại được theo thể loại và quốc gia</t>
+  </si>
+  <si>
+    <t>đã lấy được dữ liệu từ database</t>
+  </si>
+  <si>
+    <t>đàng thực hiện</t>
+  </si>
+  <si>
+    <t>chưa làm kịp</t>
   </si>
 </sst>
 </file>
@@ -2808,10 +2817,10 @@
   <dimension ref="A1:EL120"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="18" ySplit="10" topLeftCell="CU11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="18" ySplit="10" topLeftCell="CU17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="W1" sqref="W1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="CU3" sqref="CU3:CW3"/>
+      <selection pane="bottomRight" activeCell="P31" sqref="P31:P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.625" defaultRowHeight="15" customHeight="1"/>
@@ -2950,7 +2959,7 @@
       <c r="P2" s="117"/>
       <c r="Q2" s="178">
         <f ca="1">TODAY()</f>
-        <v>43296</v>
+        <v>43304</v>
       </c>
       <c r="R2" s="179"/>
       <c r="S2" s="34"/>
@@ -3106,12 +3115,12 @@
       <c r="EK2" s="39"/>
       <c r="EL2" s="15" t="str">
         <f ca="1">"Date："&amp;TEXT(TODAY()," yyyy/mm/dd")</f>
-        <v>Date： 2018/07/15</v>
+        <v>Date： 2018/07/23</v>
       </c>
     </row>
     <row r="3" spans="1:142" ht="18.75" customHeight="1">
       <c r="B3" s="140" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="121"/>
       <c r="E3" s="128"/>
@@ -3226,7 +3235,7 @@
       <c r="CJ3" s="143"/>
       <c r="CK3" s="143"/>
       <c r="CL3" s="143" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="CM3" s="143"/>
       <c r="CN3" s="143"/>
@@ -3236,27 +3245,27 @@
       <c r="CP3" s="143"/>
       <c r="CQ3" s="143"/>
       <c r="CR3" s="143" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="CS3" s="143"/>
       <c r="CT3" s="143"/>
       <c r="CU3" s="143" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="CV3" s="143"/>
       <c r="CW3" s="143"/>
       <c r="CX3" s="143" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="CY3" s="143"/>
       <c r="CZ3" s="143"/>
       <c r="DA3" s="143" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="DB3" s="143"/>
       <c r="DC3" s="143"/>
       <c r="DD3" s="143" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="DE3" s="143"/>
       <c r="DF3" s="143"/>
@@ -4769,7 +4778,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="146" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G11" s="150"/>
       <c r="H11" s="150">
@@ -5411,7 +5420,7 @@
         <v>3</v>
       </c>
       <c r="F15" s="146" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G15" s="150"/>
       <c r="H15" s="150">
@@ -6007,10 +6016,10 @@
     </row>
     <row r="19" spans="2:142" ht="9" customHeight="1">
       <c r="B19" s="207" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="199" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19" s="158">
         <v>5</v>
@@ -6038,7 +6047,9 @@
       <c r="M19" s="156"/>
       <c r="N19" s="154"/>
       <c r="O19" s="156"/>
-      <c r="P19" s="146"/>
+      <c r="P19" s="146" t="s">
+        <v>84</v>
+      </c>
       <c r="Q19" s="164"/>
       <c r="R19" s="160"/>
       <c r="S19" s="83"/>
@@ -6323,7 +6334,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="146" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G21" s="150"/>
       <c r="H21" s="150">
@@ -6343,7 +6354,7 @@
       <c r="N21" s="154"/>
       <c r="O21" s="156"/>
       <c r="P21" s="146" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="Q21" s="164"/>
       <c r="R21" s="160"/>
@@ -6617,10 +6628,10 @@
     </row>
     <row r="23" spans="2:142" ht="9" customHeight="1">
       <c r="B23" s="207" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" s="199" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" s="158">
         <v>7</v>
@@ -6629,7 +6640,7 @@
         <v>3</v>
       </c>
       <c r="F23" s="146" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G23" s="150"/>
       <c r="H23" s="150">
@@ -6649,7 +6660,7 @@
       <c r="N23" s="154"/>
       <c r="O23" s="156"/>
       <c r="P23" s="146" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q23" s="164"/>
       <c r="R23" s="160"/>
@@ -6923,10 +6934,10 @@
     </row>
     <row r="25" spans="2:142" ht="9" customHeight="1">
       <c r="B25" s="207" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C25" s="199" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" s="158">
         <v>8</v>
@@ -6948,7 +6959,9 @@
       <c r="M25" s="156"/>
       <c r="N25" s="154"/>
       <c r="O25" s="156"/>
-      <c r="P25" s="146"/>
+      <c r="P25" s="146" t="s">
+        <v>85</v>
+      </c>
       <c r="Q25" s="164"/>
       <c r="R25" s="160"/>
       <c r="S25" s="83"/>
@@ -7221,10 +7234,10 @@
     </row>
     <row r="27" spans="2:142" ht="9" customHeight="1">
       <c r="B27" s="207" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="199" t="s">
         <v>72</v>
-      </c>
-      <c r="C27" s="199" t="s">
-        <v>73</v>
       </c>
       <c r="D27" s="158">
         <v>9</v>
@@ -7519,10 +7532,10 @@
     </row>
     <row r="29" spans="2:142" ht="9" customHeight="1">
       <c r="B29" s="207" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" s="199" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D29" s="158">
         <v>10</v>
@@ -7544,7 +7557,9 @@
       <c r="M29" s="156"/>
       <c r="N29" s="154"/>
       <c r="O29" s="156"/>
-      <c r="P29" s="146"/>
+      <c r="P29" s="146" t="s">
+        <v>86</v>
+      </c>
       <c r="Q29" s="164"/>
       <c r="R29" s="160"/>
       <c r="S29" s="83"/>
@@ -7817,10 +7832,10 @@
     </row>
     <row r="31" spans="2:142" ht="9" customHeight="1">
       <c r="B31" s="207" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="199" t="s">
         <v>75</v>
-      </c>
-      <c r="C31" s="199" t="s">
-        <v>76</v>
       </c>
       <c r="D31" s="158">
         <v>11</v>
@@ -8115,7 +8130,7 @@
     </row>
     <row r="33" spans="2:142" ht="9" customHeight="1">
       <c r="B33" s="207" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C33" s="199" t="s">
         <v>57</v>
@@ -8413,7 +8428,7 @@
     </row>
     <row r="35" spans="2:142" ht="9" customHeight="1">
       <c r="B35" s="207" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C35" s="199" t="s">
         <v>52</v>

</xml_diff>